<commit_message>
style: improve Mac/Safari compatibility and contrast
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -637,6 +637,41 @@
         <v>172.5</v>
       </c>
       <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>رافعات التحدي</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>مذكرات 100 حبة - شد 50 طباعة وجه واحد</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>500</v>
+      </c>
+      <c r="F7" t="n">
+        <v>75</v>
+      </c>
+      <c r="G7" t="n">
+        <v>575</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI/UX: Edit-in-form workflow, Cancel button, row click fix, update/delete logic, and bug fixes. Refactored edit mode, improved error handling, and ensured correct transaction form state. Backend: DELETE endpoint, update mapping, and Excel fixes.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Purchases" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Expenses" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Received" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Received" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Purchases" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Expenses" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -52,7 +53,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -415,17 +416,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.28515625" customWidth="1" min="3" max="3"/>
-    <col width="12.7109375" customWidth="1" min="8" max="8"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -477,269 +474,259 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>رافعات التحدي</t>
+          <t>رحاب الزهراني</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>أبواك فواتير</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>20250515</t>
+          <t>#1: كروت | Qty: 500 | Price: 0.26 | Total: 130 | VAT: 19.5</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>500</v>
+        <v>130</v>
       </c>
       <c r="F2" t="n">
-        <v>75</v>
+        <v>19.5</v>
       </c>
       <c r="G2" t="n">
-        <v>575</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Scanned the bill,Registered in the system,Paid?,Registered the payment in the systemaa</t>
-        </is>
+        <v>149.5</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>فوفو</t>
+          <t>بشاير فلين</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>طباعة</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>11245</t>
+          <t>#1: فلين 70*50 | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">قبل و بعد </t>
+          <t>الاء الزهراني</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">نوت بوك -ايه 5- 100 حبه </t>
+          <t>#1: نوت  | Qty: 20 | Price: 10 | Total: 200 | VAT: 0</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="F4" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>690</v>
+        <v>200</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>عميل جديد</t>
+          <t>عبدالله عبدالرحمن</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>رول أب</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>#1: نص فلين | Qty: 1 | Price: 60 | Total: 60 | VAT: 0</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="F5" t="n">
-        <v>22.5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>172.5</v>
+        <v>60</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">حمد الغامدي </t>
+          <t xml:space="preserve">ديل اوت </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">ورق خطابات فاخر -100 حبه </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
+          <t>#1: ستد صرف  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: سند قبض  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #3: سند تسليم  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>150</v>
+        <v>620</v>
       </c>
       <c r="F6" t="n">
-        <v>27.5</v>
+        <v>93</v>
       </c>
       <c r="G6" t="n">
-        <v>177.5</v>
+        <v>713</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FMG</t>
+          <t xml:space="preserve">جمعية قمم </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-18</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>certificates</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>99</v>
+          <t>#1: دروع  | Qty: 4 | Price: 160 | Total: 640 | VAT: 96</t>
+        </is>
       </c>
       <c r="E7" t="n">
-        <v>200</v>
+        <v>640</v>
       </c>
       <c r="F7" t="n">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="G7" t="n">
-        <v>230</v>
+        <v>736</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">فهد باحارثه </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>#1: كوبونات عدد 1000 | Qty: 20 | Price: 18 | Total: 360 | VAT: 54</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>360</v>
+      </c>
+      <c r="F8" t="n">
+        <v>54</v>
+      </c>
+      <c r="G8" t="n">
+        <v>414</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>رافعات التحدي</t>
+          <t xml:space="preserve">بصمة الجود </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>مذكرات 100 حبة - شد 50 طباعة وجه واحد</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>150</t>
+          <t>#1: ورق خطابات 100 حبه  | Qty: 100 | Price: 1.40 | Total: 140 | VAT: 21; #2: ختم  | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="F9" t="n">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G9" t="n">
-        <v>575</v>
+        <v>299</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>123</t>
+          <t xml:space="preserve">غدي </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-05-25</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>nothing</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12345</t>
+          <t>#1: استيكرات ورقيه  | Qty: 20 | Price: 3 | Total: 60 | VAT: 9</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -748,37 +735,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>تجربے کار</t>
+          <t xml:space="preserve">سواعد العقارية </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-05-29</t>
+          <t>2025-07-16</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>تجربة طلب .. الرجاء حذفه وعدم اعتماده</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0124</t>
+          <t>#1: ورق خطابات | Qty: 2000 | Price: 0.65 | Total: 1300 | VAT: 195</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>1300</v>
       </c>
       <c r="F11" t="n">
-        <v>1.5</v>
+        <v>195</v>
       </c>
       <c r="G11" t="n">
-        <v>11.5</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Paid?</t>
-        </is>
+        <v>1495</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -787,27 +764,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>تجربي كار</t>
+          <t>تجربة عميل 1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-05-29</t>
+          <t>2025-07-18</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>قيمة كتب</t>
+          <t>#1: سندات أبواك | Qty: 10 | Price: 20 | Total: 200 | VAT: 30</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="F12" t="n">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="G12" t="n">
-        <v>575</v>
+        <v>230</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -816,32 +793,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ش</t>
+          <t>تجربة عميل 2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-05-29</t>
+          <t>2025-07-17</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>سبسش</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>12541</t>
+          <t>#1:  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>57.5</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -850,233 +822,31 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>تجربة عميل 3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-05-30</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>saf</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>5454</t>
-        </is>
-      </c>
+          <t>#1: مفكرة | Qty: 10 | Price: 14 | Total: 140 | VAT: 21</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="F14" t="n">
-        <v>0.75</v>
+        <v>21</v>
       </c>
       <c r="G14" t="n">
-        <v>5.75</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Abu Saeed (Mac)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025-05-30</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>#1: Cards | Qty: 100 | Price: 0.8 | Total: 80 | VAT: 12; #2: Stickers | Qty: 100 | Price: .55 | Total: 55.00000000000001 | VAT: 8.25</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>135</v>
-      </c>
-      <c r="F15" t="n">
-        <v>20.25</v>
-      </c>
-      <c r="G15" t="n">
-        <v>155.25</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Abu Saeed</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2025-05-30</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>#1: Books | Qty: 130 | Price: 17 | Total: 2210 | VAT: 331.5</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Quotation#237, QB#4838</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>2210</v>
-      </c>
-      <c r="F16" t="n">
-        <v>331.5</v>
-      </c>
-      <c r="G16" t="n">
-        <v>2541.5</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Abu Saeed</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2025-05-30</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>#1: Cards | Qty: 200 | Price: .5 | Total: 100 | VAT: 15; #2: Stickers | Qty: 500 | Price: .4 | Total: 200 | VAT: 30</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Quotation#272, QB#4480</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>300</v>
-      </c>
-      <c r="F17" t="n">
-        <v>45</v>
-      </c>
-      <c r="G17" t="n">
-        <v>345</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Abu Saeed</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2025-05-21</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>#1: كتاب ٢١ صفحة دبوس وسط | Qty: 100 | Price: 15 | Total: 1500 | VAT: 0; #2: استيكرات دايكت | Qty: 100 | Price: .5 | Total: 50 | VAT: 0</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Quotation#280, QB#4550</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>1550</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1550</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>abu saeed</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2025-05-30</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>#1: books again | Qty: 10 | Price: 54 | Total: 540 | VAT: 81</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>540</v>
-      </c>
-      <c r="F19" t="n">
-        <v>81</v>
-      </c>
-      <c r="G19" t="n">
-        <v>621</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Registered in QB,Paid</t>
-        </is>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>testing Paid amount</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2025-06-01</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>#1: item one | Qty: 1 | Price: 100 | Total: 100 | VAT: 15; #2: Item two | Qty: 2 | Price: 75 | Total: 150 | VAT: 22.5</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>250</v>
-      </c>
-      <c r="F20" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="G20" t="n">
-        <v>287.5</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Registered in QB,Paid,Paid,Paid,Paid:full</t>
-        </is>
-      </c>
-      <c r="I20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1091,7 +861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,77 +882,28 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>Notes</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Method</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>VAT</t>
+          <t>Actions</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Actions</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
           <t>Done</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>بلب الورق</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-05-15</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ورق 150 جرام لأديف</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>644</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2" t="n">
-        <v>115</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Scanned the bill,Registered in the system,Paid?,Registered the payment in the system</t>
-        </is>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +920,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1262,10 +983,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1283,61 +1004,38 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>VAT</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>Actions</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Done</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Abu Saeed</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-05-30</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>224</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>as</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Recorded in Journal,Recorded in QB</t>
-        </is>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Auto-focus description field when editing a single-item sales transaction, not just multi-item.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,7 +835,6 @@
           <t>#1: مفكرة | Qty: 10 | Price: 14 | Total: 140 | VAT: 21</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>140</v>
       </c>
@@ -845,8 +844,38 @@
       <c r="G14" t="n">
         <v>161</v>
       </c>
-      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>تجربة عميل4</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>#1: بروش | Qty: 2 | Price: 20 | Total: 40 | VAT: 6</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>40</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" t="n">
+        <v>46</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature: Add sort options and clickable table header arrows for Name, Date, Amount, Done, Reference, and Total. Reset sort on Clear button.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,7 +864,6 @@
           <t>#1: بروش | Qty: 2 | Price: 20 | Total: 40 | VAT: 6</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>40</v>
       </c>
@@ -874,8 +873,67 @@
       <c r="G15" t="n">
         <v>46</v>
       </c>
-      <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>مركز  كنز الطفوله</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>#1: سند قبض  | Qty: 20 | Price: 20 | Total: 400 | VAT: 60</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>400</v>
+      </c>
+      <c r="F16" t="n">
+        <v>60</v>
+      </c>
+      <c r="G16" t="n">
+        <v>460</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عجائب للاسماك </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>#1: فواتير بي فايف  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>220</v>
+      </c>
+      <c r="F17" t="n">
+        <v>33</v>
+      </c>
+      <c r="G17" t="n">
+        <v>253</v>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Edit/Delete now use unique _rowIdx for each transaction, ensuring correct row is targeted after filtering or sorting.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Expenses" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -53,7 +52,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -416,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -474,466 +473,2212 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>رحاب الزهراني</t>
+          <t>رافعات التحدي</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>#1: كروت | Qty: 500 | Price: 0.26 | Total: 130 | VAT: 19.5</t>
+          <t>أبواك فواتير</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20250515</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>130</v>
+        <v>500</v>
       </c>
       <c r="F2" t="n">
-        <v>19.5</v>
+        <v>75</v>
       </c>
       <c r="G2" t="n">
-        <v>149.5</v>
+        <v>575</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Scanned the bill,Registered in the system,Paid?,Registered the payment in the systemaa</t>
+        </is>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>بشاير فلين</t>
+          <t>فوفو</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>#1: فلين 70*50 | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
+          <t>طباعة</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11245</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G3" t="n">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>الاء الزهراني</t>
+          <t xml:space="preserve">قبل و بعد </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>#1: نوت  | Qty: 20 | Price: 10 | Total: 200 | VAT: 0</t>
+          <t xml:space="preserve">نوت بوك -ايه 5- 100 حبه </t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G4" t="n">
-        <v>200</v>
+        <v>690</v>
       </c>
       <c r="I4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>عبدالله عبدالرحمن</t>
+          <t>عميل جديد</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>#1: نص فلين | Qty: 1 | Price: 60 | Total: 60 | VAT: 0</t>
+          <t>رول أب</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
+        <v>172.5</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">ديل اوت </t>
+          <t xml:space="preserve">حمد الغامدي </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>#1: ستد صرف  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: سند قبض  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #3: سند تسليم  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
+          <t xml:space="preserve">ورق خطابات فاخر -100 حبه </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>620</v>
+        <v>150</v>
       </c>
       <c r="F6" t="n">
-        <v>93</v>
+        <v>27.5</v>
       </c>
       <c r="G6" t="n">
-        <v>713</v>
+        <v>177.5</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">جمعية قمم </t>
+          <t>FMG</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-05-18</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>#1: دروع  | Qty: 4 | Price: 160 | Total: 640 | VAT: 96</t>
-        </is>
+          <t>certificates</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>99</v>
       </c>
       <c r="E7" t="n">
-        <v>640</v>
+        <v>200</v>
       </c>
       <c r="F7" t="n">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="G7" t="n">
-        <v>736</v>
+        <v>230</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">فهد باحارثه </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-07-10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>#1: كوبونات عدد 1000 | Qty: 20 | Price: 18 | Total: 360 | VAT: 54</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>360</v>
-      </c>
-      <c r="F8" t="n">
-        <v>54</v>
-      </c>
-      <c r="G8" t="n">
-        <v>414</v>
-      </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">بصمة الجود </t>
+          <t>رافعات التحدي</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>#1: ورق خطابات 100 حبه  | Qty: 100 | Price: 1.40 | Total: 140 | VAT: 21; #2: ختم  | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+          <t>مذكرات 100 حبة - شد 50 طباعة وجه واحد</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>150</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>260</v>
+        <v>500</v>
       </c>
       <c r="F9" t="n">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="G9" t="n">
-        <v>299</v>
+        <v>575</v>
       </c>
       <c r="I9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">غدي </t>
+          <t>123</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-05-25</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>#1: استيكرات ورقيه  | Qty: 20 | Price: 3 | Total: 60 | VAT: 9</t>
+          <t>nothing</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>12345</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F10" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">سواعد العقارية </t>
+          <t>تجربے کار</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-07-16</t>
+          <t>2025-05-29</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>#1: ورق خطابات | Qty: 2000 | Price: 0.65 | Total: 1300 | VAT: 195</t>
+          <t>تجربة طلب .. الرجاء حذفه وعدم اعتماده</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0124</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1300</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>195</v>
+        <v>1.5</v>
       </c>
       <c r="G11" t="n">
-        <v>1495</v>
+        <v>11.5</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Paid?</t>
+        </is>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>تجربة عميل 1</t>
+          <t>تجربي كار</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-07-18</t>
+          <t>2025-05-29</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>#1: سندات أبواك | Qty: 10 | Price: 20 | Total: 200 | VAT: 30</t>
+          <t>قيمة كتب</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F12" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="G12" t="n">
-        <v>230</v>
+        <v>575</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>تجربة عميل 2</t>
+          <t>ش</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-07-17</t>
+          <t>2025-05-29</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>#1:  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+          <t>سبسش</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12541</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>57.5</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>تجربة عميل 3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>#1: مفكرة | Qty: 10 | Price: 14 | Total: 140 | VAT: 21</t>
+          <t>saf</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5454</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>21</v>
+        <v>0.75</v>
       </c>
       <c r="G14" t="n">
-        <v>161</v>
+        <v>5.75</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>تجربة عميل4</t>
+          <t>Abu Saeed (Mac)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-07-18</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>#1: بروش | Qty: 2 | Price: 20 | Total: 40 | VAT: 6</t>
+          <t>#1: Cards | Qty: 100 | Price: 0.8 | Total: 80 | VAT: 12; #2: Stickers | Qty: 100 | Price: .55 | Total: 55.00000000000001 | VAT: 8.25</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="F15" t="n">
-        <v>6</v>
+        <v>20.25</v>
       </c>
       <c r="G15" t="n">
-        <v>46</v>
+        <v>155.25</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>مركز  كنز الطفوله</t>
+          <t>Abu Saeed</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-07-21</t>
+          <t>2025-05-30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>#1: سند قبض  | Qty: 20 | Price: 20 | Total: 400 | VAT: 60</t>
+          <t>#1: Books | Qty: 130 | Price: 17 | Total: 2210 | VAT: 331.5</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Quotation#237, QB#4838</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>400</v>
+        <v>2210</v>
       </c>
       <c r="F16" t="n">
-        <v>60</v>
+        <v>331.5</v>
       </c>
       <c r="G16" t="n">
-        <v>460</v>
+        <v>2541.5</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Abu Saeed</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>#1: Cards | Qty: 200 | Price: .5 | Total: 100 | VAT: 15; #2: Stickers | Qty: 500 | Price: .4 | Total: 200 | VAT: 30</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Quotation#272, QB#4480</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>300</v>
+      </c>
+      <c r="F17" t="n">
+        <v>45</v>
+      </c>
+      <c r="G17" t="n">
+        <v>345</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Abu Saeed</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-05-21</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>#1: كتاب ٢١ صفحة دبوس وسط | Qty: 100 | Price: 15 | Total: 1500 | VAT: 0; #2: استيكرات دايكت | Qty: 100 | Price: .5 | Total: 50 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Quotation#280, QB#4550</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1550</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1550</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>abu saeed</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>#1: books again | Qty: 10 | Price: 54 | Total: 540 | VAT: 81</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>540</v>
+      </c>
+      <c r="F19" t="n">
+        <v>81</v>
+      </c>
+      <c r="G19" t="n">
+        <v>621</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Registered in QB,Paid</t>
+        </is>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>testing Paid amount</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>#1: item one | Qty: 1 | Price: 100 | Total: 100 | VAT: 15; #2: Item two | Qty: 2 | Price: 75 | Total: 150 | VAT: 22.5</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>250</v>
+      </c>
+      <c r="F20" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>287.5</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Registered in QB,Paid,Paid,Paid,Paid:full</t>
+        </is>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>#1: استيكرات قهوة راواندا | Qty: 150 | Price: .3 | Total: 45 | VAT: 0; #2: كتب مدارس الأقصى | Qty: 150 | Price: 15 | Total: 2250 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Quotation#</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2295</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2295</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">البيت الطبي </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>#1: بطاقة اي دي ورق مقوى  | Qty: 2 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">البيت الطبي </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>#1: بطاقة اي دي ورق مقوى  | Qty: 2 | Price: 15 | Total: 30 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Invoice#287.290, QB#4856</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>30</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>30</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Registered in QB</t>
+        </is>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">محمد عرب </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>#1:  مقاس a4 استيكرات على فوركس  | Qty: 18 | Price: 0 | Total: 0 | VAT: 0; #2: استيكرات a4  | Qty: 4 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">سلاف - فتحي القرشي </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>#1: ختم دائري  | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>120</v>
+      </c>
+      <c r="F25" t="n">
+        <v>18</v>
+      </c>
+      <c r="G25" t="n">
+        <v>138</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">نواف بابطين </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>#1: بطائق ورق مقوى - مقاس a6  | Qty: 25 | Price: 1.60 | Total: 40 | VAT: 6</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>40</v>
+      </c>
+      <c r="F26" t="n">
+        <v>6</v>
+      </c>
+      <c r="G26" t="n">
+        <v>46</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ام عبدالمحسن </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>#1: طباعة ورق عادي  | Qty: 54 | Price: 0.5 | Total: 27 | VAT: 4.05</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>27</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="G27" t="n">
+        <v>31.05</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ام عبدالمحسن </t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>#1: طباعة بطاقة a6 | Qty: 11 | Price: 1 | Total: 11 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>11</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>11</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>الوحدة للحديد</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>#1: أبواك فواتير - مقاس كبير - أصل + 2 نسخة | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: ختم دائري كبير للشركة | Qty: 1 | Price: 120 | Total: 120 | VAT: 18; #3: أورقا خطاب | Qty: 1 | Price: 150 | Total: 150 | VAT: 22.5</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>470</v>
+      </c>
+      <c r="F29" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>540.5</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Registered in QB,Paid,Paid,Paid,Paid,Paid,Paid:full</t>
+        </is>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عبدالله الزهراني </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>#1: لوحه اكريليك مقاس 30*30 | Qty: 2 | Price: 90 | Total: 180 | VAT: 27; #2: لوحه اكريليك مقاس 90*60 | Qty: 1 | Price: 300 | Total: 300 | VAT: 45; #3: لوجه اكريليك مقاس 36*46 | Qty: 1 | Price: 99 | Total: 99 | VAT: 14.85</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>579</v>
+      </c>
+      <c r="F30" t="n">
+        <v>86.84999999999999</v>
+      </c>
+      <c r="G30" t="n">
+        <v>665.85</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>صالح الغامدي</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>#1: ختم دائري  | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>120</v>
+      </c>
+      <c r="F31" t="n">
+        <v>18</v>
+      </c>
+      <c r="G31" t="n">
+        <v>138</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">سما النسيم </t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>#1: برشور A5 | Qty: 500 | Price: 0.5 | Total: 250 | VAT: 37.5</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>250</v>
+      </c>
+      <c r="F32" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="G32" t="n">
+        <v>287.5</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">سما النسيم </t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>#1: 500 برشور A5 | Qty: 500 | Price: 0.8 | Total: 400 | VAT: 60; #2: تصمم مينو A3 مع طباعة 5 اوراق  | Qty: 1 | Price: 200 | Total: 200 | VAT: 30</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>600</v>
+      </c>
+      <c r="F33" t="n">
+        <v>90</v>
+      </c>
+      <c r="G33" t="n">
+        <v>690</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">دستيك </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-06-04</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>#1: ختم مستطيل  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>بشائر الزعتري</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>#1: استيكرات مربع 3*3 سم إن دور | Qty: 500 | Price: .69 | Total: 345 | VAT: 0; #2: توصيل | Qty: 1 | Price: 35 | Total: 35 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>QB#4868</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>380</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>380</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Registered in QB,Paid,Paid,Paid:full</t>
+        </is>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- عرض سعر -باسم - الفاضل </t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>#1: لوحه اكريليك 6 ملي مقاس 40*30 مع نسمارين==مسمارين  | Qty: 1 | Price: 170 | Total: 170 | VAT: 25.5; #2: برشور a4 مطوي طيه واحدة  | Qty: 500 | Price: 0.80 | Total: 400 | VAT: 60; #3: تصميم مينو  | Qty: 1 | Price: 300 | Total: 300 | VAT: 45</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>870</v>
+      </c>
+      <c r="F36" t="n">
+        <v>130.5</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1000.5</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">موسسة مولدات المتحدة </t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>#1: بزنس كارد 1000 | Qty: 1 | Price: 160 | Total: 160 | VAT: 24; #2: استيكر مقاس 20*30  | Qty: 100 | Price: 4.20 | Total: 420 | VAT: 63</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>580</v>
+      </c>
+      <c r="F37" t="n">
+        <v>87</v>
+      </c>
+      <c r="G37" t="n">
+        <v>667</v>
+      </c>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">مصنع بلاستيك جدة </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>#1: تغير استيكر مقاس 100*100 | Qty: 1 | Price: 150 | Total: 150 | VAT: 22.5</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>150</v>
+      </c>
+      <c r="F38" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="G38" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-02-26</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>#1: منيو  | Qty: 10 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>#1: استيكر  | Qty: 5000 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-04-17</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>#1: استيكر صيانه  | Qty: 2 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>#1: استيكرات  | Qty: 5000 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>#1: استيكر شفاف  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>#1: لوحه اكريليك  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>#1: استيكر باب  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شاي فال </t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>#1: استيكر  | Qty: 5000 | Price: 0 | Total: 0 | VAT: 0; #2: منيو  | Qty: 20 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عم هاشم </t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>#1: كوبانات عدد 12دفتر - الشده 50 | Qty: 12 | Price: 18 | Total: 216 | VAT: 32.4; #2: تركيب مكعبات  | Qty: 3 | Price: 100 | Total: 300 | VAT: 45; #3: طباعة مطويه -3 طيات  | Qty: 500 | Price: 1.20 | Total: 600 | VAT: 90</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>1116</v>
+      </c>
+      <c r="F47" t="n">
+        <v>167.4</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1283.4</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ياسر فضالي </t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>#1: جلده ختم  | Qty: 1 | Price: 40 | Total: 40 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>40</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>40</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">كريم </t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-06-21</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>#1: بزنس كارد  | Qty: 200 | Price: 0.50 | Total: 100 | VAT: 15</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>100</v>
+      </c>
+      <c r="F49" t="n">
+        <v>15</v>
+      </c>
+      <c r="G49" t="n">
+        <v>115</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">حامد القرني </t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>#1: استيكر مفرغ  | Qty: 4 | Price: 60 | Total: 240 | VAT: 36; #2: لوحه فورسكس مقاس a3- 3m | Qty: 4 | Price: 30 | Total: 120 | VAT: 18; #3: توصيل  | Qty: 1 | Price: 40 | Total: 40 | VAT: 6</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>400</v>
+      </c>
+      <c r="F50" t="n">
+        <v>60</v>
+      </c>
+      <c r="G50" t="n">
+        <v>460</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">جمعية قمم </t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-06-24</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس اي فايف  | Qty: 10 | Price: 3 | Total: 30 | VAT: 4.5; #2: بزنس كارد  | Qty: 100 | Price: 0.80 | Total: 80 | VAT: 12; #3: اي دي كرت  | Qty: 1 | Price: 50 | Total: 50 | VAT: 7.5</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>160</v>
+      </c>
+      <c r="F51" t="n">
+        <v>24</v>
+      </c>
+      <c r="G51" t="n">
+        <v>184</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">الشركة المتحدة- عرض سعر </t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>#1: فولدر - جيب واحد  | Qty: 100 | Price: 6 | Total: 600 | VAT: 90; #2: نوت جلدي  | Qty: 100 | Price: 12 | Total: 1200 | VAT: 180; #3: قلم  | Qty: 100 | Price: 7 | Total: 700 | VAT: 105; #4: بروفايل 9 صفحات  | Qty: 100 | Price: 5 | Total: 500 | VAT: 75; #5: بروفايل 28 صفحة  | Qty: 100 | Price: 12 | Total: 1200 | VAT: 180; #6: بروفايل 43 صفحة  | Qty: 100 | Price: 25 | Total: 2500 | VAT: 375; #7: كيس قماشي مقاس a4 | Qty: 100 | Price: 16 | Total: 1600 | VAT: 240; #8: كوستر  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>8300</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1245</v>
+      </c>
+      <c r="G52" t="n">
+        <v>9545</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">حديد الغريبه </t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>#1: لوحة اكريلك a3 | Qty: 1 | Price: 200 | Total: 200 | VAT: 30; #2: بزنس كارد  | Qty: 300 | Price: 1 | Total: 300 | VAT: 45; #3: ختم  | Qty: 2 | Price: 120 | Total: 240 | VAT: 36</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>740</v>
+      </c>
+      <c r="F53" t="n">
+        <v>111</v>
+      </c>
+      <c r="G53" t="n">
+        <v>851</v>
+      </c>
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">عبدالرحمن الحربي </t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 6*6 | Qty: 100 | Price: 1.8 | Total: 180 | VAT: 0; #2:  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>180</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>180</v>
+      </c>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">قبل و بعد </t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>#1: لوحة اسم  | Qty: 1 | Price: 1 | Total: 1 | VAT: 0.15; #2: لوحه باب  | Qty: 1 | Price: 1 | Total: 1 | VAT: 0.15; #3: اورق A4 | Qty: 6 | Price: 1 | Total: 6 | VAT: 0.9</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>8</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G55" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>شركة محترفي التنظيم</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>#1: ورق خطابات | Qty: 100 | Price: 1.5 | Total: 150 | VAT: 22.5; #2: ختم | Qty: 1 | Price: 138 | Total: 138 | VAT: 20.7</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>288</v>
+      </c>
+      <c r="F56" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="G56" t="n">
+        <v>331.2</v>
+      </c>
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>مرام</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>#1: استاند مائي | Qty: 72 | Price: 30 | Total: 2160 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>2160</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2160</v>
+      </c>
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">شركة وصل </t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-06-29</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس ٦٠*٣٤ | Qty: 20 | Price: 20 | Total: 400 | VAT: 60</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>400</v>
+      </c>
+      <c r="F58" t="n">
+        <v>60</v>
+      </c>
+      <c r="G58" t="n">
+        <v>460</v>
+      </c>
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>رحاب الزهراني</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025-07-05</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>#1: كروت | Qty: 500 | Price: 0.26 | Total: 130 | VAT: 19.5</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>130</v>
+      </c>
+      <c r="F59" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="G59" t="n">
+        <v>149.5</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>بشاير فلين</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2025-07-05</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>#1: فلين 70*50 | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>50</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>50</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>الاء الزهراني</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-07-05</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>#1: نوت  | Qty: 20 | Price: 10 | Total: 200 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>200</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>200</v>
+      </c>
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>عبدالله عبدالرحمن</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-07-05</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>#1: نص فلين | Qty: 1 | Price: 60 | Total: 60 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>60</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>60</v>
+      </c>
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ديل اوت </t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2025-07-09</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>#1: ستد صرف  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: سند قبض  | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #3: سند تسليم  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>620</v>
+      </c>
+      <c r="F63" t="n">
+        <v>93</v>
+      </c>
+      <c r="G63" t="n">
+        <v>713</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">جمعية قمم </t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2025-07-09</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>#1: دروع  | Qty: 4 | Price: 160 | Total: 640 | VAT: 96</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>640</v>
+      </c>
+      <c r="F64" t="n">
+        <v>96</v>
+      </c>
+      <c r="G64" t="n">
+        <v>736</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">فهد باحارثه </t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>#1: كوبونات عدد 1000 | Qty: 20 | Price: 18 | Total: 360 | VAT: 54</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>360</v>
+      </c>
+      <c r="F65" t="n">
+        <v>54</v>
+      </c>
+      <c r="G65" t="n">
+        <v>414</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">بصمة الجود </t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>#1: ورق خطابات 100 حبه  | Qty: 100 | Price: 1.40 | Total: 140 | VAT: 21; #2: ختم  | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>260</v>
+      </c>
+      <c r="F66" t="n">
+        <v>39</v>
+      </c>
+      <c r="G66" t="n">
+        <v>299</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">غدي </t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>#1: استيكرات ورقيه  | Qty: 20 | Price: 3 | Total: 60 | VAT: 9</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>60</v>
+      </c>
+      <c r="F67" t="n">
+        <v>9</v>
+      </c>
+      <c r="G67" t="n">
+        <v>69</v>
+      </c>
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">سواعد العقارية </t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>#1: ورق خطابات | Qty: 2000 | Price: 0.65 | Total: 1300 | VAT: 195</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F68" t="n">
+        <v>195</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1495</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>تجربة عميل 1</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>#1: سندات أبواك | Qty: 10 | Price: 20 | Total: 200 | VAT: 30</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>200</v>
+      </c>
+      <c r="F69" t="n">
+        <v>30</v>
+      </c>
+      <c r="G69" t="n">
+        <v>230</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>تجربة عميل 2</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>#1:  | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>تجربة عميل 3</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>#1: مفكرة | Qty: 10 | Price: 14 | Total: 140 | VAT: 21</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>140</v>
+      </c>
+      <c r="F71" t="n">
+        <v>21</v>
+      </c>
+      <c r="G71" t="n">
+        <v>161</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>تجربة عميل4</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-07-18</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>#1: بروش | Qty: 2 | Price: 20 | Total: 40 | VAT: 6</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>40</v>
+      </c>
+      <c r="F72" t="n">
+        <v>6</v>
+      </c>
+      <c r="G72" t="n">
+        <v>46</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>مركز  كنز الطفوله</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-07-21</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>#1: سند قبض | Qty: 20 | Price: 20 | Total: 400 | VAT: 60</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>QB#5041</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>400</v>
+      </c>
+      <c r="F73" t="n">
+        <v>60</v>
+      </c>
+      <c r="G73" t="n">
+        <v>460</v>
+      </c>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t xml:space="preserve">عجائب للاسماك </t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>2025-07-21</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>#1: فواتير بي فايف  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
+      <c r="E74" t="n">
         <v>220</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F74" t="n">
         <v>33</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G74" t="n">
         <v>253</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="b">
+      <c r="I74" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI: Set constant width for Actions column to fit Edit and Delete icons side by side, ensuring consistent layout.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -3765,7 +3765,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Quotation#177</t>
+          <t>Quotation#177, QB#614</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -3794,7 +3794,12 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>#1: ورق خطابات | Qty: 200 | Price: 01.2 | Total: 240 | VAT: 0; #2: استيكرات Titan ASD 200 | Qty: 500 | Price: 1.85 | Total: 925 | VAT: 0; #3: استيكرات SpectraGuard 225 | Qty: 200 | Price: 1.85 | Total: 370 | VAT: 0; #4: استيكرات SpectraGuard 300 | Qty: 100 | Price: 1.85 | Total: 185 | VAT: 0; #5: استيكرات SpectraGuard 360 | Qty: 100 | Price: 1.85 | Total: 185 | VAT: 0</t>
+          <t>#1: ورق خطابات | Qty: 200 | Price: 1.2 | Total: 240 | VAT: 0; #2: استيكرات Titan ASD 200 | Qty: 500 | Price: 1.85 | Total: 925 | VAT: 0; #3: استيكرات SpectraGuard 225 | Qty: 200 | Price: 1.85 | Total: 370 | VAT: 0; #4: استيكرات SpectraGuard 300 | Qty: 100 | Price: 1.85 | Total: 185 | VAT: 0; #5: استيكرات SpectraGuard 360 | Qty: 100 | Price: 1.85 | Total: 185 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>QB#5076</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -3826,6 +3831,11 @@
           <t>#1: استيكرات القهوة متفرقة | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
         </is>
       </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>QB#5077</t>
+        </is>
+      </c>
       <c r="E111" t="n">
         <v>0</v>
       </c>
@@ -3855,6 +3865,11 @@
           <t>#1: نوت بوك كالعادة | Qty: 10 | Price: 10 | Total: 100 | VAT: 0</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>QB#5078</t>
+        </is>
+      </c>
       <c r="E112" t="n">
         <v>100</v>
       </c>
@@ -3864,6 +3879,7 @@
       <c r="G112" t="n">
         <v>100</v>
       </c>
+      <c r="H112" t="inlineStr"/>
       <c r="I112" t="b">
         <v>0</v>
       </c>
@@ -3942,7 +3958,6 @@
           <t>#1: ورق الخطابات | Qty: 100 | Price: 1.4 | Total: 140 | VAT: 21; #2: أظرف A4 | Qty: 200 | Price: 2.5 | Total: 500 | VAT: 75; #3: أظرف DL | Qty: 200 | Price: 1.8 | Total: 360 | VAT: 54; #4: فولدر مطبوع وجهين مع جيب واحد | Qty: 100 | Price: 7.2 | Total: 720 | VAT: 108; #5: نوت بوك A6 تقفيل غراء - شد 30 ورقة | Qty: 100 | Price: 6 | Total: 600 | VAT: 90; #6: لوحة أكريليك مقاس 60*40 سم - مع 4 مسامير ألمنيوم | Qty: 1 | Price: 200 | Total: 200 | VAT: 30</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr"/>
       <c r="E115" t="n">
         <v>2520</v>
       </c>
@@ -3952,7 +3967,6 @@
       <c r="G115" t="n">
         <v>2898</v>
       </c>
-      <c r="H115" t="inlineStr"/>
       <c r="I115" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Branding: Set favicon to Logo-icon.svg for improved tab icon.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
@@ -3879,7 +3879,6 @@
       <c r="G112" t="n">
         <v>100</v>
       </c>
-      <c r="H112" t="inlineStr"/>
       <c r="I112" t="b">
         <v>0</v>
       </c>
@@ -3900,6 +3899,11 @@
           <t>#1: بروشور مقاس A5 وجهين | Qty: 100 | Price: 1.5 | Total: 150 | VAT: 0</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>QB#5079</t>
+        </is>
+      </c>
       <c r="E113" t="n">
         <v>150</v>
       </c>
@@ -3968,6 +3972,124 @@
         <v>2898</v>
       </c>
       <c r="I115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>خبراء الفلاتر</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>2025-07-28</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>#1: استيكر منتج - طباعة ديجيتال - مقاس 10*15 سم | Qty: 100 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>شاي فال</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>2025-07-28</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>#1: استيكرات النظافة - بلاش على قولة سامي | Qty: 5 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>مجمع قبل وبعد</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2025-07-28</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>#1: بطاقات آي دي موظفين | Qty: 3 | Price: 28 | Total: 84 | VAT: 12.6</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>84</v>
+      </c>
+      <c r="F118" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="G118" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="I118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>روافد القهوة</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 24*13 سم - طباعة ديجيتال - مع سلوفان مطفي | Qty: 150 | Price: 1 | Total: 150 | VAT: 22.5</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="n">
+        <v>150</v>
+      </c>
+      <c r="F119" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="G119" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI polish: Add horizontal logo to app header, update button and checkbox checked states to use theme colors, and improve overall branding.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1107,7 +1107,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>#1: بطاقة اي دي ورق مقوى  | Qty: 2 | Price: 0 | Total: 0 | VAT: 0</t>
+          <t>#1: بطاقة اي دي ورق مقوى | Qty: 2 | Price: 0 | Total: 0 | VAT: 0</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1170,9 +1170,10 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>#1:  مقاس a4 استيكرات على فوركس  | Qty: 18 | Price: 0 | Total: 0 | VAT: 0; #2: استيكرات a4  | Qty: 4 | Price: 0 | Total: 0 | VAT: 0</t>
-        </is>
-      </c>
+          <t>#1: مقاس a4 استيكرات على فوركس | Qty: 18 | Price: 0 | Total: 0 | VAT: 0; #2: استيكرات a4 | Qty: 4 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>0</v>
       </c>
@@ -1182,8 +1183,9 @@
       <c r="G24" t="n">
         <v>0</v>
       </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -4078,7 +4080,6 @@
           <t>#1: استيكر مقاس 24*13 سم - طباعة ديجيتال - مع سلوفان مطفي | Qty: 150 | Price: 1 | Total: 150 | VAT: 22.5</t>
         </is>
       </c>
-      <c r="D119" t="inlineStr"/>
       <c r="E119" t="n">
         <v>150</v>
       </c>
@@ -4088,7 +4089,6 @@
       <c r="G119" t="n">
         <v>172.5</v>
       </c>
-      <c r="H119" t="inlineStr"/>
       <c r="I119" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
UI polish: Stack logo above title and center header, add spacing between Update/Cancel, fix Clear button alignment/hover, theme scroll-to-top button, and apply brand color to Edit/Delete icons.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1173,7 +1173,6 @@
           <t>#1: مقاس a4 استيكرات على فوركس | Qty: 18 | Price: 0 | Total: 0 | VAT: 0; #2: استيكرات a4 | Qty: 4 | Price: 0 | Total: 0 | VAT: 0</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>0</v>
       </c>
@@ -1183,7 +1182,6 @@
       <c r="G24" t="n">
         <v>0</v>
       </c>
-      <c r="H24" t="inlineStr"/>
       <c r="I24" t="b">
         <v>1</v>
       </c>
@@ -2972,7 +2970,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>#1: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18; #2: ورق خطابات فاخر | Qty: 100 | Price: 1.5 | Total: 150 | VAT: 22.5</t>
+          <t>#1: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18; #2: ورق خطابات فاخر | Qty: 1000 | Price: .85 | Total: 850 | VAT: 127.5; #3: أظرف مقاس A4 | Qty: 1000 | Price: 1.4 | Total: 1400 | VAT: 210</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2981,14 +2979,15 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>270</v>
+        <v>2370</v>
       </c>
       <c r="F84" t="n">
-        <v>40.5</v>
+        <v>355.5</v>
       </c>
       <c r="G84" t="n">
-        <v>310.5</v>
-      </c>
+        <v>2725.5</v>
+      </c>
+      <c r="H84" t="inlineStr"/>
       <c r="I84" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fix: Force table header background and text color with !important to ensure visibility and brand styling.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>QB#5052</t>
+          <t>Invoice#348, QB#5052</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2749,6 +2749,7 @@
       <c r="G77" t="n">
         <v>51.75</v>
       </c>
+      <c r="H77" t="inlineStr"/>
       <c r="I77" t="b">
         <v>0</v>
       </c>
@@ -2987,7 +2988,6 @@
       <c r="G84" t="n">
         <v>2725.5</v>
       </c>
-      <c r="H84" t="inlineStr"/>
       <c r="I84" t="b">
         <v>0</v>
       </c>
@@ -4089,6 +4089,282 @@
         <v>172.5</v>
       </c>
       <c r="I119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>علي عمر دين</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>#1: أكريليك استاند إي فور مع ثنية | Qty: 1 | Price: 35 | Total: 35 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>35</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>35</v>
+      </c>
+      <c r="I120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>علا للمصاعد</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>#1: سند صيانة | Qty: 50 | Price: 13 | Total: 650 | VAT: 97.5</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>650</v>
+      </c>
+      <c r="F121" t="n">
+        <v>97.5</v>
+      </c>
+      <c r="G121" t="n">
+        <v>747.5</v>
+      </c>
+      <c r="I121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>رائد - كابلات بحرة</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>#1: ختم بيضاوي 3045 | Qty: 1 | Price: 140 | Total: 140 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>QB#5083</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>140</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>140</v>
+      </c>
+      <c r="I122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>شاي فال</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>#1: منيو بوخار | Qty: 10 | Price: 10 | Total: 100 | VAT: 15; #2: منيو شاي فال | Qty: 10 | Price: 2.75 | Total: 27.5 | VAT: 4.13; #3: كرت افتتاح فرع 9.5*13.5 سم | Qty: 500 | Price: 0.6 | Total: 300 | VAT: 45; #4: أكريليك مقاس 35*60 سم | Qty: 2 | Price: 250 | Total: 500 | VAT: 75</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>QB#50845085</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>927.5</v>
+      </c>
+      <c r="F123" t="n">
+        <v>139.13</v>
+      </c>
+      <c r="G123" t="n">
+        <v>1066.63</v>
+      </c>
+      <c r="I123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>#1: استيكرات قهوة متنوع | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>محمد المالكي UK صاحب صهيب</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>#1: طباعة كيس ورقي للهدايا | Qty: 3 | Price: 25 | Total: 75 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>75</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" t="n">
+        <v>75</v>
+      </c>
+      <c r="I125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>عبدالله السندي - صاحب عمر</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2025-07-29</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>#1: طباعة ورق إي ثري ديجيتال - بلاش | Qty: 3 | Price: 0 | Total: 0 | VAT: 0; #2: بنر مقاس 50*70 سم | Qty: 1 | Price: 40 | Total: 40 | VAT: 0; #3: بروشور 150 جرام A5 طباعة وجهين | Qty: 100 | Price: 1.2 | Total: 120 | VAT: 0; #4: فلين مقاس 100*70 سم | Qty: 2 | Price: 75 | Total: 150 | VAT: 0; #5: فلين مقاس 50*50 سم | Qty: 5 | Price: 40 | Total: 200 | VAT: 0; #6: خصم 10 ريال | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>510</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" t="n">
+        <v>510</v>
+      </c>
+      <c r="I126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>البروج الذهبية</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>#1: تصميم الهوية | Qty: 1 | Price: 304.35 | Total: 304.35 | VAT: 45.65; #2: طباعة فولدر مقاس A4 - طباعة جهة واحدة - بجيب داخلي واحد على اليسار | Qty: 100 | Price: 5 | Total: 500 | VAT: 75; #3: طباعة ورق الخطابات كونكورر فاخر | Qty: 500 | Price: .8 | Total: 400 | VAT: 60; #4: طباعة ورق الخطابات وودفري | Qty: 500 | Price: .6 | Total: 300 | VAT: 45; #5: طباعة ظرف A4 وجه واحد | Qty: 200 | Price: 2.6 | Total: 520 | VAT: 78; #6: طباعة ظرف A5 وجه واحد | Qty: 200 | Price: 2.2 | Total: 440.00000000000006 | VAT: 66; #7: طباعة ظرف DL وجه واحد | Qty: 200 | Price: 1.8 | Total: 360 | VAT: 54; #8: طباعة سندات قبض - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #9: طباعة سندات صرف - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #10: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Quotation#194, Invoice#347</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>3304.35</v>
+      </c>
+      <c r="F127" t="n">
+        <v>495.65</v>
+      </c>
+      <c r="G127" t="n">
+        <v>3800</v>
+      </c>
+      <c r="I127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>شركة كيري</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2025-07-30</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>#1: ختم دائري R538 | Qty: 2 | Price: 120 | Total: 240 | VAT: 36</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>240</v>
+      </c>
+      <c r="F128" t="n">
+        <v>36</v>
+      </c>
+      <c r="G128" t="n">
+        <v>276</v>
+      </c>
+      <c r="I128" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI polish, branding, and bugfixes: themed Done checkmark, fixed Show Done Transactions logic, improved table layout, and prepared for Received Amount tab bugfixing
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" state="visible" r:id="rId1"/>
@@ -415,9 +415,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>#1: استيكرات قهوة راواندا | Qty: 150 | Price: .3 | Total: 45 | VAT: 0; #2: كتب مدارس الأقصى | Qty: 150 | Price: 15 | Total: 2250 | VAT: 0</t>
+          <t>#1: استيكرات قهوة راواندا | Qty: 150 | Price: 0.3 | Total: 45 | VAT: 0; #2: كتب مدارس الأقصى | Qty: 150 | Price: 15 | Total: 2250 | VAT: 0</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1091,7 +1091,7 @@
         <v>2295</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>#1: بطائق ورق مقوى - مقاس a6  | Qty: 25 | Price: 1.60 | Total: 40 | VAT: 6</t>
+          <t>#1: بطائق ورق مقوى - مقاس a6 | Qty: 25 | Price: 1.6 | Total: 40 | VAT: 6</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1241,7 +1241,7 @@
         <v>46</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -2749,7 +2749,6 @@
       <c r="G77" t="n">
         <v>51.75</v>
       </c>
-      <c r="H77" t="inlineStr"/>
       <c r="I77" t="b">
         <v>0</v>
       </c>
@@ -3034,22 +3033,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>#1: فوركس 1ملم - مع طباعة مقاس 100*200 سم - | Qty: 4 | Price: 250 | Total: 1000 | VAT: 150</t>
+          <t>#1: فوركس 1ملم - مع طباعة مقاس 100*200 سم - | Qty: 5 | Price: 320 | Total: 1600 | VAT: 240; #2: فوركس 1ملم - مع طباعة مقاس 112*144 سم - | Qty: 5 | Price: 250 | Total: 1250 | VAT: 187.5</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>QB#5059</t>
+          <t>Quotation#207, QB#5059</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>1000</v>
+        <v>2850</v>
       </c>
       <c r="F86" t="n">
-        <v>150</v>
+        <v>427.5</v>
       </c>
       <c r="G86" t="n">
-        <v>1150</v>
+        <v>3277.5</v>
       </c>
       <c r="I86" t="b">
         <v>0</v>
@@ -3107,7 +3106,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>QB#5056</t>
+          <t>QB#5057</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -3466,7 +3465,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>#1: استيكرات دائرية 4*4 سم | Qty: 1000 | Price: 0.35 | Total: 350 | VAT: 52.5; #2: استيكرات مربع 6*6 سم | Qty: 1000 | Price: 0.4 | Total: 400 | VAT: 60</t>
+          <t>#1: استيكرات دائرية شفافة - مقاس 5.5*5.5 سم | Qty: 200 | Price: .8 | Total: 160 | VAT: 0</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3475,13 +3474,13 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>750</v>
+        <v>160</v>
       </c>
       <c r="F99" t="n">
-        <v>112.5</v>
+        <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>862.5</v>
+        <v>160</v>
       </c>
       <c r="I99" t="b">
         <v>0</v>
@@ -3645,17 +3644,22 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>#1: فوركس 6 ملم مطبوع كامل الشيت | Qty: 2 | Price: 500 | Total: 1000 | VAT: 150</t>
+          <t>#1: فوركس 6 ملم مطبوع كامل الشيت | Qty: 1 | Price: 500 | Total: 500 | VAT: 75</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Invoice#352, QB#5087</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="F105" t="n">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="G105" t="n">
-        <v>1150</v>
+        <v>575</v>
       </c>
       <c r="I105" t="b">
         <v>0</v>
@@ -4365,6 +4369,1091 @@
         <v>276</v>
       </c>
       <c r="I128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>شركة ريڤايڤا</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>#1: استيكرات مقاس 50*25 سم | Qty: 6 | Price: 34.78 | Total: 208.68 | VAT: 31.3</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Invoice#352, QB#5088</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>208.68</v>
+      </c>
+      <c r="F129" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="G129" t="n">
+        <v>239.98</v>
+      </c>
+      <c r="I129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>نادي الاتحاد</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>#1: لوحات فوركس 1 ملم - مقاس 88*68 سم | Qty: 5 | Price: 200 | Total: 1000 | VAT: 150; #2: لوحات فوركس 3 ملم - مقاس 6.5*40 سم | Qty: 20 | Price: 40 | Total: 800 | VAT: 120; #3: فوركس 6 ملم - مع طباعة جهتين مقاس 38*10 سم | Qty: 3 | Price: 60 | Total: 180 | VAT: 27</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Quotation#208</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F130" t="n">
+        <v>297</v>
+      </c>
+      <c r="G130" t="n">
+        <v>2277</v>
+      </c>
+      <c r="I130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>نادي الاتحاد</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>#1: لوحة فوركس مقاس A4 - شكلين كل واحد مكرر 3 مرات - مع قاعدة أكريليك مطبوعة يو في | Qty: 6 | Price: 100 | Total: 600 | VAT: 90</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Quotation#206</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>600</v>
+      </c>
+      <c r="F131" t="n">
+        <v>90</v>
+      </c>
+      <c r="G131" t="n">
+        <v>690</v>
+      </c>
+      <c r="I131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>نادي الاتحاد</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>#1: لوحة فوركس مقاس A5 - شكلين حبة من كل واحد - مع قاعدة أكريليك مطبوعة يو في | Qty: 2 | Price: 70 | Total: 140 | VAT: 21</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Quotation#206</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>140</v>
+      </c>
+      <c r="F132" t="n">
+        <v>21</v>
+      </c>
+      <c r="G132" t="n">
+        <v>161</v>
+      </c>
+      <c r="I132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>خبراء الفلاتر</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>#1: استيكر منتج - طباعة ديجيتال - مقاس 10*15 سم | Qty: 100 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>خبراء الفلاتر</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>#1: استيكر منتج - طباعة ديجيتال - مقاس 10*15 سم | Qty: 100 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>QB#5089</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>شاي فال</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>#1: هاشتاق أكريليك مقاس 50*15 سم | Qty: 1 | Price: 100 | Total: 100 | VAT: 15; #2: هذا الطلب مأخوذ سابقاً بتاريخ 12/5/2025 اليوم طلب من جديد.. أحط رقم الفاتورة السابقة للمرجع فقط | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Invoice#309, QB#5090</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>100</v>
+      </c>
+      <c r="F135" t="n">
+        <v>15</v>
+      </c>
+      <c r="G135" t="n">
+        <v>115</v>
+      </c>
+      <c r="I135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>المحاور الأربعة - يحيى جحرة</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>#1: سندات صرف - 1+1 - طباعة لونين | Qty: 10 | Price: 27 | Total: 270 | VAT: 40.5</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Invoice#356, QB#5091</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>270</v>
+      </c>
+      <c r="F136" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="G136" t="n">
+        <v>310.5</v>
+      </c>
+      <c r="I136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>سواعد العقارية</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>#1: سندات صرف - 1+2 - لون واحد | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: توصيل | Qty: 1 | Price: 34.78 | Total: 34.78 | VAT: 5.22</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Invoice#360, QB#5092</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>234.78</v>
+      </c>
+      <c r="F137" t="n">
+        <v>35.22</v>
+      </c>
+      <c r="G137" t="n">
+        <v>270</v>
+      </c>
+      <c r="I137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>شركة مريل</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>#1: بزنس كارد ناعم الحواف - 3 نماذج - ألف من كل نموذج | Qty: 3000 | Price: 0.38 | Total: 1140 | VAT: 0; #2: تكملة فرق الضريبة | Qty: 1 | Price: 171 | Total: 171 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>QB#5093</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>1311</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0</v>
+      </c>
+      <c r="G138" t="n">
+        <v>1311</v>
+      </c>
+      <c r="I138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>توابل الجودة</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>#1: بزنس كارد | Qty: 200 | Price: 0.58 | Total: 115.99999999999999 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>116</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>116</v>
+      </c>
+      <c r="I139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>#1: استيركرات القهوة | Qty: 200 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>مجمع قبل وبعد</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>#1: كروت مقاس 12*7 سم - وجهين - بلاش | Qty: 15 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>بيت الطب</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>#1: بطاقة | Qty: 1 | Price: 13.05 | Total: 13.05 | VAT: 1.96</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Invoice#355</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="F142" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="G142" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="I142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>رسين - علا للمصاعد</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>2025-08-03</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>#1: طباعة فولدر وجه واحد مقاس إي فور - مع جيب واحد | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: استيكرات الأقسام - مفرغة مع الشعار - مقاس 40*10 سم - أسود+ذهبي | Qty: 6 | Price: 50 | Total: 300 | VAT: 45; #3: أكريليك الأقسام - مفرغة مع الشعار - مقاس 40*10 سم | Qty: 3 | Price: 80 | Total: 240 | VAT: 36</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Quotation#209</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>740</v>
+      </c>
+      <c r="F143" t="n">
+        <v>111</v>
+      </c>
+      <c r="G143" t="n">
+        <v>851</v>
+      </c>
+      <c r="I143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>معاذ سعيد</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>2025-08-03</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>#1: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 3.5*1 سم | Qty: 2000 | Price: .18 | Total: 360 | VAT: 0; #2: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 7*3 سم | Qty: 500 | Price: .48 | Total: 240 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>600</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>600</v>
+      </c>
+      <c r="I144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>سواعد العقارية</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>#1: سندات صرف - 1+2 - لون واحد | Qty: 10 | Price: 20 | Total: 200 | VAT: 30; #2: توصيل | Qty: 1 | Price: 34.78 | Total: 34.78 | VAT: 5.22</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Invoice#360, QB#5092</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>234.78</v>
+      </c>
+      <c r="F145" t="n">
+        <v>35.22</v>
+      </c>
+      <c r="G145" t="n">
+        <v>270</v>
+      </c>
+      <c r="I145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>مؤسسة ديار أمجاد للمقاولات</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>#1: تعديل تصميم ورق الخطابات | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>50</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="n">
+        <v>50</v>
+      </c>
+      <c r="I146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>كيان للمحاماة - بلال الرفاعي</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>2025-08-03</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>#1: طباعة كروت آي دي من قبل العميل | Qty: 6 | Price: 25 | Total: 150 | VAT: 22.5</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Invoice#357</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>150</v>
+      </c>
+      <c r="F147" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="G147" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="I147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>قلوس كراج - Gloss Garage</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>#1: بروشور A5 - طباعة وجه واحد | Qty: 100 | Price: 1.72 | Total: 172 | VAT: 0; #2: توصيل | Qty: 1 | Price: 40.5 | Total: 40.5 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="I148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>أم عبدالمحسن</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>#1: كروت A5 - طباعة وجه واحد | Qty: 200 | Price: .5 | Total: 100 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>100</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>100</v>
+      </c>
+      <c r="I149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>سليمان حمود - صاحب عمر</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 5.5*13.5 سم - طباعة ديجيتال | Qty: 100 | Price: 1.03 | Total: 103 | VAT: 0; #2: سليف علبة - طباعة ورق 150 جرام - مقاس 21*6.5 سم | Qty: 100 | Price: 2.07 | Total: 206.99999999999997 | VAT: 0; #3: تسوية الضريبة | Qty: 1 | Price: .5 | Total: 0.5 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>310.5</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>310.5</v>
+      </c>
+      <c r="I150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>سليمان حمود - صاحب عمر</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>#1: توريد وطباعة أكياس ورقية - مقاس A5 | Qty: 100 | Price: 3.45 | Total: 345 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>345</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>345</v>
+      </c>
+      <c r="I151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>علي العطاس</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>#1: كتب لوبريف - 100 ورقة - تغليف فاخر | Qty: 50 | Price: 110 | Total: 5500 | VAT: 825</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>5500</v>
+      </c>
+      <c r="F152" t="n">
+        <v>825</v>
+      </c>
+      <c r="G152" t="n">
+        <v>6325</v>
+      </c>
+      <c r="I152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>مركز الطبي الدولي</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>#1: اعتماد درع وسط لـ Qadar Zada | Qty: 1 | Price: 280 | Total: 280 | VAT: 42</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>280</v>
+      </c>
+      <c r="F153" t="n">
+        <v>42</v>
+      </c>
+      <c r="G153" t="n">
+        <v>322</v>
+      </c>
+      <c r="I153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>لانا فلين</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>#1: فلين مقاس 70*100 سم - مطبوع وجه واحد | Qty: 2 | Price: 80 | Total: 160 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>160</v>
+      </c>
+      <c r="F154" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" t="n">
+        <v>160</v>
+      </c>
+      <c r="I154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>أجاد</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>#1: استيكر الأدهم - شفاف - مقاس 3*2 سم | Qty: 100 | Price: .75 | Total: 75 | VAT: 0; #2: استيكر الكميت - شفاف - مقاس 3*2 سم | Qty: 100 | Price: .75 | Total: 75 | VAT: 0; #3: كرت طريقة الاستخدام - كوشيه مسلفن مطفي - مقاس A6 - طباعة وجهين | Qty: 500 | Price: .51 | Total: 255 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>405</v>
+      </c>
+      <c r="F155" t="n">
+        <v>0</v>
+      </c>
+      <c r="G155" t="n">
+        <v>405</v>
+      </c>
+      <c r="I155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>مؤسسة معاذ الشعيبي</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>#1: ختم دائري مقاس R538 | Qty: 1 | Price: 115 | Total: 115 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>115</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="n">
+        <v>115</v>
+      </c>
+      <c r="I156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>مطعم سما النسيم</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>#1: تعديل منيو | Qty: 1 | Price: 150 | Total: 150 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>150</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>150</v>
+      </c>
+      <c r="I157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>أسامة الجميعي</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>#1: ختم R538 | Qty: 1 | Price: 138 | Total: 138 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>138</v>
+      </c>
+      <c r="F158" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" t="n">
+        <v>138</v>
+      </c>
+      <c r="I158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>شاي فال</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>#1: هاشتاق أكريليك - طلب من جديد | Qty: 1 | Price: 100 | Total: 100 | VAT: 15</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>100</v>
+      </c>
+      <c r="F159" t="n">
+        <v>15</v>
+      </c>
+      <c r="G159" t="n">
+        <v>115</v>
+      </c>
+      <c r="I159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>روضة حنان الورد</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>#1: سندات قبض | Qty: 10 | Price: 23 | Total: 230 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>230</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>230</v>
+      </c>
+      <c r="I160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>إيهاب الحاج</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>#1: طباعة على فلين مقاس 50*70 سم | Qty: 1 | Price: 46 | Total: 46 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>46</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>46</v>
+      </c>
+      <c r="I161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>كابلات بحرة</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>#1: ختم صغير Abdullah Abad AlManamy | Qty: 1 | Price: 50 | Total: 50 | VAT: 7.5</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Invoice#362</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>50</v>
+      </c>
+      <c r="F162" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G162" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="I162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>#1: استيكرات القهوة | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>0</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4379,10 +5468,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4422,6 +5511,277 @@
         <is>
           <t>Done</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>150</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">قيمة أكواب قهوة
+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>لارين</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>سلامات</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>كابلات بحرة</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>تالين</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>150</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>150</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>سالم دواليب</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-06-28</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>70</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>قيمة دواليب خربانة</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>عطية الزهراني</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>مركز صح</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes for Received Amount tab: update-in-place, notes/method display, done status, robust edit/cancel, removed Total column, fixed Show Done Transactions toggle
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -5468,7 +5468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -5544,11 +5544,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -5773,15 +5773,60 @@
       <c r="C12" t="n">
         <v>30</v>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>cash</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
       <c r="G12" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>400</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-06-07</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>250</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>bank</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sales form improvements: moved discount to overall sale, fixed price input for decimals, restored totals, ensured backend receives discount, cleared discount after save/update, removed discount from item form, fixed type errors, and improved UX for price entry. All changes from today included.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Expenses" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -415,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177:XFD178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2601,7 +2601,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>#1: فواتير بي فايف  | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
+          <t>#1: فواتير بي فايف | Qty: 10 | Price: 22 | Total: 220 | VAT: 33</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>QB#5037</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2703,7 +2708,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>QB#5054</t>
+          <t>QB#5053</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -3337,6 +3342,11 @@
           <t>#1: كتيب A5 - 12 صفحة | Qty: 400 | Price: 9 | Total: 3600 | VAT: 540</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Quotation#197</t>
+        </is>
+      </c>
       <c r="E95" t="n">
         <v>3600</v>
       </c>
@@ -3531,6 +3541,11 @@
           <t>#1: بنر مقاس 100*100 سم | Qty: 1 | Price: 40 | Total: 40 | VAT: 0</t>
         </is>
       </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>QB#5134</t>
+        </is>
+      </c>
       <c r="E101" t="n">
         <v>40</v>
       </c>
@@ -3615,7 +3630,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>#1: بنر مقاس 150*100 سم  | Qty: 3 | Price: 60 | Total: 180 | VAT: 0</t>
+          <t>#1: بنر مقاس 150*100 سم | Qty: 3 | Price: 60 | Total: 180 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>QB#5135</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -3649,7 +3669,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Invoice#352, QB#5087</t>
+          <t>Invoice#350, QB#5087</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -3681,6 +3701,11 @@
           <t>#1: استيكر مفرغ مع تركيب على السيارة جهتين | Qty: 1 | Price: 150 | Total: 150 | VAT: 22.5</t>
         </is>
       </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Invoice#349, QB#5143</t>
+        </is>
+      </c>
       <c r="E106" t="n">
         <v>150</v>
       </c>
@@ -3707,7 +3732,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>#1: كروت مسلفنة | Qty: 1000 | Price: .15 | Total: 150 | VAT: 0</t>
+          <t>#1: كروت مسلفنة | Qty: 1000 | Price: 0.15 | Total: 150 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>QB#5138</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -3736,7 +3766,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>#1: استيكر دائري 5*5 سم - 01 | Qty: 250 | Price: 0.35 | Total: 87.5 | VAT: 0; #2: استيكر دائري 5*5 سم - 02 | Qty: 750 | Price: 0.35 | Total: 262.5 | VAT: 0; #3: استيكر دائري 5*5 سم - B | Qty: 200 | Price: 0.6 | Total: 120 | VAT: 0; #4: استيكر دائري 5*5 سم - M | Qty: 150 | Price: 0.62 | Total: 93 | VAT: 0; #5: استيكر دائري 5*5 سم - G | Qty: 100 | Price: .62 | Total: 62 | VAT: 0</t>
+          <t>#1: استيكر دائري 5*5 سم - 01 | Qty: 250 | Price: 0.35 | Total: 87.5 | VAT: 0; #2: استيكر دائري 5*5 سم - 02 | Qty: 750 | Price: 0.35 | Total: 262.5 | VAT: 0; #3: استيكر دائري 5*5 سم - B | Qty: 200 | Price: 0.6 | Total: 120 | VAT: 0; #4: استيكر دائري 5*5 سم - M | Qty: 150 | Price: 0.62 | Total: 93 | VAT: 0; #5: استيكر دائري 5*5 سم - G | Qty: 100 | Price: 0.62 | Total: 62 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>QB#5137</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -3938,6 +3973,11 @@
           <t>#1: كتاب 12 صفحة تغليف سلك | Qty: 1 | Price: 40 | Total: 40 | VAT: 0; #2: شهادات | Qty: 2 | Price: 5 | Total: 10 | VAT: 0</t>
         </is>
       </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>QB#5141</t>
+        </is>
+      </c>
       <c r="E114" t="n">
         <v>50</v>
       </c>
@@ -3964,17 +4004,22 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>#1: ورق الخطابات | Qty: 100 | Price: 1.4 | Total: 140 | VAT: 21; #2: أظرف A4 | Qty: 200 | Price: 2.5 | Total: 500 | VAT: 75; #3: أظرف DL | Qty: 200 | Price: 1.8 | Total: 360 | VAT: 54; #4: فولدر مطبوع وجهين مع جيب واحد | Qty: 100 | Price: 7.2 | Total: 720 | VAT: 108; #5: نوت بوك A6 تقفيل غراء - شد 30 ورقة | Qty: 100 | Price: 6 | Total: 600 | VAT: 90; #6: لوحة أكريليك مقاس 60*40 سم - مع 4 مسامير ألمنيوم | Qty: 1 | Price: 200 | Total: 200 | VAT: 30</t>
+          <t>#1: ورق الخطابات | Qty: 100 | Price: 1.61 | Total: 161 | VAT: 0; #2: أظرف A4 | Qty: 200 | Price: 2.87 | Total: 574 | VAT: 0; #3: أظرف DL | Qty: 200 | Price: 2.07 | Total: 413.99999999999994 | VAT: 0; #4: فولدر مطبوع وجهين مع جيب واحد | Qty: 100 | Price: 8.28 | Total: 827.9999999999999 | VAT: 0; #5: نوت بوك A6 تقفيل غراء - شد 30 ورقة | Qty: 100 | Price: 6.9 | Total: 690 | VAT: 0; #6: لوحة أكريليك مقاس 60*40 سم - مع 4 مسامير ألمنيوم | Qty: 1 | Price: 230 | Total: 230 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>QB#5133</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>2520</v>
+        <v>2897</v>
       </c>
       <c r="F115" t="n">
-        <v>378</v>
+        <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="I115" t="b">
         <v>0</v>
@@ -4083,6 +4128,11 @@
           <t>#1: استيكر مقاس 24*13 سم - طباعة ديجيتال - مع سلوفان مطفي | Qty: 150 | Price: 1 | Total: 150 | VAT: 22.5</t>
         </is>
       </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Quotation#202, QB#5142</t>
+        </is>
+      </c>
       <c r="E119" t="n">
         <v>150</v>
       </c>
@@ -4254,7 +4304,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>محمد المالكي UK صاحب صهيب</t>
+          <t>محمد الزهراني UK صاحب صهيب</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4265,6 +4315,11 @@
       <c r="C125" t="inlineStr">
         <is>
           <t>#1: طباعة كيس ورقي للهدايا | Qty: 3 | Price: 25 | Total: 75 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>QB#5139</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -4296,6 +4351,11 @@
           <t>#1: طباعة ورق إي ثري ديجيتال - بلاش | Qty: 3 | Price: 0 | Total: 0 | VAT: 0; #2: بنر مقاس 50*70 سم | Qty: 1 | Price: 40 | Total: 40 | VAT: 0; #3: بروشور 150 جرام A5 طباعة وجهين | Qty: 100 | Price: 1.2 | Total: 120 | VAT: 0; #4: فلين مقاس 100*70 سم | Qty: 2 | Price: 75 | Total: 150 | VAT: 0; #5: فلين مقاس 50*50 سم | Qty: 5 | Price: 40 | Total: 200 | VAT: 0; #6: خصم 10 ريال | Qty: 1 | Price: 0 | Total: 0 | VAT: 0</t>
         </is>
       </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>QB#5140</t>
+        </is>
+      </c>
       <c r="E126" t="n">
         <v>510</v>
       </c>
@@ -4322,12 +4382,12 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>#1: تصميم الهوية | Qty: 1 | Price: 304.35 | Total: 304.35 | VAT: 45.65; #2: طباعة فولدر مقاس A4 - طباعة جهة واحدة - بجيب داخلي واحد على اليسار | Qty: 100 | Price: 5 | Total: 500 | VAT: 75; #3: طباعة ورق الخطابات كونكورر فاخر | Qty: 500 | Price: .8 | Total: 400 | VAT: 60; #4: طباعة ورق الخطابات وودفري | Qty: 500 | Price: .6 | Total: 300 | VAT: 45; #5: طباعة ظرف A4 وجه واحد | Qty: 200 | Price: 2.6 | Total: 520 | VAT: 78; #6: طباعة ظرف A5 وجه واحد | Qty: 200 | Price: 2.2 | Total: 440.00000000000006 | VAT: 66; #7: طباعة ظرف DL وجه واحد | Qty: 200 | Price: 1.8 | Total: 360 | VAT: 54; #8: طباعة سندات قبض - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #9: طباعة سندات صرف - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #10: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+          <t>#1: تصميم الهوية | Qty: 1 | Price: 304.35 | Total: 304.35 | VAT: 45.65; #2: طباعة فولدر مقاس A4 - طباعة جهة واحدة - بجيب داخلي واحد على اليسار | Qty: 100 | Price: 5 | Total: 500 | VAT: 75; #3: طباعة ورق الخطابات كونكورر فاخر | Qty: 500 | Price: 0.8 | Total: 400 | VAT: 60; #4: طباعة ورق الخطابات وودفري | Qty: 500 | Price: 0.6 | Total: 300 | VAT: 45; #5: طباعة ظرف A4 وجه واحد | Qty: 200 | Price: 2.6 | Total: 520 | VAT: 78; #6: طباعة ظرف A5 وجه واحد | Qty: 200 | Price: 2.2 | Total: 440.00000000000006 | VAT: 66; #7: طباعة ظرف DL وجه واحد | Qty: 200 | Price: 1.8 | Total: 360 | VAT: 54; #8: طباعة سندات قبض - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #9: طباعة سندات صرف - لون واحد - 1+2 | Qty: 10 | Price: 18 | Total: 180 | VAT: 27; #10: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Quotation#194, Invoice#347</t>
+          <t>Quotation#194, Invoice#347, QB#5150</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -4403,7 +4463,7 @@
         <v>239.98</v>
       </c>
       <c r="I129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -4723,6 +4783,11 @@
           <t>#1: بزنس كارد | Qty: 200 | Price: 0.58 | Total: 115.99999999999999 | VAT: 0</t>
         </is>
       </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>QB#5161</t>
+        </is>
+      </c>
       <c r="E139" t="n">
         <v>116</v>
       </c>
@@ -4733,7 +4798,7 @@
         <v>116</v>
       </c>
       <c r="I139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -4812,7 +4877,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Invoice#355</t>
+          <t>Invoice#355, QB#5160</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -4825,7 +4890,7 @@
         <v>15.01</v>
       </c>
       <c r="I142" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -4875,7 +4940,12 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>#1: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 3.5*1 سم | Qty: 2000 | Price: .18 | Total: 360 | VAT: 0; #2: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 7*3 سم | Qty: 500 | Price: .48 | Total: 240 | VAT: 0</t>
+          <t>#1: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 3.5*1 سم | Qty: 2000 | Price: 0.18 | Total: 360 | VAT: 0; #2: استيكر باركود - طباعة ديجيتال - قص دايكت - مقاس 7*3 سم | Qty: 500 | Price: 0.48 | Total: 240 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>QB#5159</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -4888,7 +4958,7 @@
         <v>600</v>
       </c>
       <c r="I144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -4941,6 +5011,11 @@
           <t>#1: تعديل تصميم ورق الخطابات | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
         </is>
       </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>QB#5163</t>
+        </is>
+      </c>
       <c r="E146" t="n">
         <v>50</v>
       </c>
@@ -4972,7 +5047,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Invoice#357</t>
+          <t>Invoice#357, QB#5157</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -5030,7 +5105,12 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>#1: كروت A5 - طباعة وجه واحد | Qty: 200 | Price: .5 | Total: 100 | VAT: 0</t>
+          <t>#1: كروت A5 - طباعة وجه واحد | Qty: 200 | Price: 0.5 | Total: 100 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>QB#5162</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -5059,7 +5139,12 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>#1: استيكر مقاس 5.5*13.5 سم - طباعة ديجيتال | Qty: 100 | Price: 1.03 | Total: 103 | VAT: 0; #2: سليف علبة - طباعة ورق 150 جرام - مقاس 21*6.5 سم | Qty: 100 | Price: 2.07 | Total: 206.99999999999997 | VAT: 0; #3: تسوية الضريبة | Qty: 1 | Price: .5 | Total: 0.5 | VAT: 0</t>
+          <t>#1: استيكر مقاس 5.5*13.5 سم - طباعة ديجيتال | Qty: 100 | Price: 1.03 | Total: 103 | VAT: 0; #2: سليف علبة - طباعة ورق 150 جرام - مقاس 21*6.5 سم | Qty: 100 | Price: 2.07 | Total: 207 | VAT: 0; #3: تسوية الضريبة | Qty: 1 | Price: 0.5 | Total: 0.5 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>QB#5165</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -5088,17 +5173,22 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>#1: توريد وطباعة أكياس ورقية - مقاس A5 | Qty: 100 | Price: 3.45 | Total: 345 | VAT: 0</t>
+          <t>#1: توريد وطباعة أكياس ورقية - مقاس A5 | Qty: 100 | Price: 3.45 | Total: 345 | VAT: 0; #2: استيكر مقاس 5*5 سم - دائري | Qty: 100 | Price: .69 | Total: 69 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>QB#5165</t>
         </is>
       </c>
       <c r="E151" t="n">
-        <v>345</v>
+        <v>414</v>
       </c>
       <c r="F151" t="n">
         <v>0</v>
       </c>
       <c r="G151" t="n">
-        <v>345</v>
+        <v>414</v>
       </c>
       <c r="I151" t="b">
         <v>0</v>
@@ -5117,17 +5207,22 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>#1: كتب لوبريف - 100 ورقة - تغليف فاخر | Qty: 50 | Price: 110 | Total: 5500 | VAT: 825</t>
+          <t>#1: كتب لوبريف - 100 ورقة - تغليف فاخر | Qty: 52 | Price: 144 | Total: 7488 | VAT: 1123.2</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Quotation#214, Invoice#374</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>5500</v>
+        <v>7488</v>
       </c>
       <c r="F152" t="n">
-        <v>825</v>
+        <v>1123.2</v>
       </c>
       <c r="G152" t="n">
-        <v>6325</v>
+        <v>8611.200000000001</v>
       </c>
       <c r="I152" t="b">
         <v>0</v>
@@ -5178,6 +5273,11 @@
           <t>#1: فلين مقاس 70*100 سم - مطبوع وجه واحد | Qty: 2 | Price: 80 | Total: 160 | VAT: 0</t>
         </is>
       </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>QB#5164</t>
+        </is>
+      </c>
       <c r="E154" t="n">
         <v>160</v>
       </c>
@@ -5188,7 +5288,7 @@
         <v>160</v>
       </c>
       <c r="I154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -5204,18 +5304,20 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>#1: استيكر الأدهم - شفاف - مقاس 3*2 سم | Qty: 100 | Price: .75 | Total: 75 | VAT: 0; #2: استيكر الكميت - شفاف - مقاس 3*2 سم | Qty: 100 | Price: .75 | Total: 75 | VAT: 0; #3: كرت طريقة الاستخدام - كوشيه مسلفن مطفي - مقاس A6 - طباعة وجهين | Qty: 500 | Price: .51 | Total: 255 | VAT: 0</t>
-        </is>
-      </c>
+          <t>#1: استيكر الأدهم - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.745 | Total: 74.5 | VAT: 0; #2: استيكر الكميت - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.745 | Total: 74.5 | VAT: 0; #3: استيكر مقاس 5.5*5.5 سم - دائري | Qty: 200 | Price: 0.805 | Total: 161 | VAT: 0; #4: كرت طريقة الاستخدام - كوشيه مسلفن مطفي - مقاس A6 - طباعة وجهين | Qty: 500 | Price: 0.506 | Total: 253 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
       <c r="E155" t="n">
-        <v>405</v>
+        <v>563</v>
       </c>
       <c r="F155" t="n">
         <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>405</v>
-      </c>
+        <v>550</v>
+      </c>
+      <c r="H155" t="inlineStr"/>
       <c r="I155" t="b">
         <v>0</v>
       </c>
@@ -5265,6 +5367,11 @@
           <t>#1: تعديل منيو | Qty: 1 | Price: 150 | Total: 150 | VAT: 0</t>
         </is>
       </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>QB#5121</t>
+        </is>
+      </c>
       <c r="E157" t="n">
         <v>150</v>
       </c>
@@ -5294,6 +5401,11 @@
           <t>#1: ختم R538 | Qty: 1 | Price: 138 | Total: 138 | VAT: 0</t>
         </is>
       </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>QB#5122</t>
+        </is>
+      </c>
       <c r="E158" t="n">
         <v>138</v>
       </c>
@@ -5323,6 +5435,11 @@
           <t>#1: هاشتاق أكريليك - طلب من جديد | Qty: 1 | Price: 100 | Total: 100 | VAT: 15</t>
         </is>
       </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>QB#5123</t>
+        </is>
+      </c>
       <c r="E159" t="n">
         <v>100</v>
       </c>
@@ -5352,6 +5469,11 @@
           <t>#1: سندات قبض | Qty: 10 | Price: 23 | Total: 230 | VAT: 0</t>
         </is>
       </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>QB#5124</t>
+        </is>
+      </c>
       <c r="E160" t="n">
         <v>230</v>
       </c>
@@ -5381,6 +5503,11 @@
           <t>#1: طباعة على فلين مقاس 50*70 سم | Qty: 1 | Price: 46 | Total: 46 | VAT: 0</t>
         </is>
       </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>QB#5125</t>
+        </is>
+      </c>
       <c r="E161" t="n">
         <v>46</v>
       </c>
@@ -5454,6 +5581,1222 @@
         <v>0</v>
       </c>
       <c r="I163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>حامد القرني - وزارة الصحة</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>2025-06-24</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>#1: طباعة بوب أب - استاند من العميل | Qty: 1 | Price: 1495 | Total: 1495 | VAT: 0; #2: رول اب مع استاند | Qty: 1 | Price: 230 | Total: 230 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>QB#5100</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>1725</v>
+      </c>
+      <c r="F164" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" t="n">
+        <v>1725</v>
+      </c>
+      <c r="I164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>معاذ السروري</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>2025-08-07</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>#1: دروع كريستال | Qty: 81 | Price: 60 | Total: 4860 | VAT: 0; #2: درع صغير - كريستال | Qty: 1 | Price: 18 | Total: 18 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>QB#5126</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>4878</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" t="n">
+        <v>4878</v>
+      </c>
+      <c r="I165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>خبراء الأخشاب</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>#1: كروت يوسف الرواشدة | Qty: 1000 | Price: .16 | Total: 160 | VAT: 24</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Invoice#364, QB#5116</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>160</v>
+      </c>
+      <c r="F166" t="n">
+        <v>24</v>
+      </c>
+      <c r="G166" t="n">
+        <v>184</v>
+      </c>
+      <c r="I166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>توارد</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>#1: ورق خطابات كونكورر مضلع وجه واحد | Qty: 200 | Price: 1.2 | Total: 240 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>QB#5117</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>240</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" t="n">
+        <v>240</v>
+      </c>
+      <c r="I167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>فارس الحربي</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 60*12 سم | Qty: 2 | Price: 20 | Total: 40 | VAT: 0; #2: استيكر مقاس 44*7 سم | Qty: 1 | Price: 10 | Total: 10 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>QB#5120</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>50</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0</v>
+      </c>
+      <c r="G168" t="n">
+        <v>50</v>
+      </c>
+      <c r="I168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>أم عبدالمحسن</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>#1: كتاب من 9 صفحات تغليف حلزوني | Qty: 1 | Price: 30 | Total: 30 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>QB#5118</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>30</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0</v>
+      </c>
+      <c r="G169" t="n">
+        <v>30</v>
+      </c>
+      <c r="I169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>مركز الطبي الدولي</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>#1: درع وسط باسم Ms. Cristina Valente | Qty: 1 | Price: 280 | Total: 280 | VAT: 42</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Invoice#363, QB#5119</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>280</v>
+      </c>
+      <c r="F170" t="n">
+        <v>42</v>
+      </c>
+      <c r="G170" t="n">
+        <v>322</v>
+      </c>
+      <c r="I170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>سعيد باسعيد</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>#1: لوحات فوركس مع قص مقاس 50*50 سم | Qty: 4 | Price: 80 | Total: 320 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>QB#5127</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>320</v>
+      </c>
+      <c r="F171" t="n">
+        <v>0</v>
+      </c>
+      <c r="G171" t="n">
+        <v>320</v>
+      </c>
+      <c r="I171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>شركة نواة الخصوصية - وفاء</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>#1: ختم مستطيل S853 | Qty: 1 | Price: 138 | Total: 138 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>QB#5132</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>138</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" t="n">
+        <v>138</v>
+      </c>
+      <c r="I172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>اجاد</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>#1: استيكر شفاف - دائري مقاس 6*6 | Qty: 240 | Price: 0.96 | Total: 230.39999999999998 | VAT: 0; #2: استيكر شفاف - مقاس 3.50*4.50 | Qty: 240 | Price: 0.67 | Total: 160.8 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>391.2</v>
+      </c>
+      <c r="F173" t="n">
+        <v>0</v>
+      </c>
+      <c r="G173" t="n">
+        <v>391.2</v>
+      </c>
+      <c r="I173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>مركز معين الصيفي</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>#1: كتيب مقاس 25*25 سم - 36 صفحة - داخلي 150 جرام - غلاف 300 جرام مسلفن مطفي - دبوس وسط | Qty: 1 | Price: 50 | Total: 50 | VAT: 0; #2: كتيب مقاس 25*25 سم - 32 صفحة - داخلي 150 جرام - غلاف 300 جرام مسلفن مطفي - دبوس وسط | Qty: 1 | Price: 50 | Total: 50 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>100</v>
+      </c>
+      <c r="F174" t="n">
+        <v>0</v>
+      </c>
+      <c r="G174" t="n">
+        <v>100</v>
+      </c>
+      <c r="I174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>خبراء الفلاتر</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>#1: كروت إحسان | Qty: 1000 | Price: .16 | Total: 160 | VAT: 24</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>160</v>
+      </c>
+      <c r="F175" t="n">
+        <v>24</v>
+      </c>
+      <c r="G175" t="n">
+        <v>184</v>
+      </c>
+      <c r="I175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>روضة حنان الورد</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 99*61 سم | Qty: 1 | Price: 60 | Total: 60 | VAT: 0; #2: توصيل | Qty: 1 | Price: 20 | Total: 20 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>80</v>
+      </c>
+      <c r="F176" t="n">
+        <v>0</v>
+      </c>
+      <c r="G176" t="n">
+        <v>80</v>
+      </c>
+      <c r="I176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>حامد القرني - وزارة الصحة</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>#1: درع كريستال مع صندوق قطيفة | Qty: 1 | Price: 170 | Total: 170 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>QB#5154</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>170</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0</v>
+      </c>
+      <c r="G177" t="n">
+        <v>170</v>
+      </c>
+      <c r="I177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>شركة سال المتحدة</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>#1: استيكر مع شيت مغناطيس مقاس 40*25 سم | Qty: 4 | Price: 50 | Total: 200 | VAT: 30</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>200</v>
+      </c>
+      <c r="F178" t="n">
+        <v>30</v>
+      </c>
+      <c r="G178" t="n">
+        <v>230</v>
+      </c>
+      <c r="I178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>مجمع قبل وبعد</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>#1: كرت العيادة | Qty: 2000 | Price: .65 | Total: 1300 | VAT: 195; #2: كرت أبو رواس | Qty: 1000 | Price: .65 | Total: 650 | VAT: 97.5; #3: كرت سلمى | Qty: 1000 | Price: .65 | Total: 650 | VAT: 97.5</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F179" t="n">
+        <v>390</v>
+      </c>
+      <c r="G179" t="n">
+        <v>2990</v>
+      </c>
+      <c r="I179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>المراحل المتقدمة - ليفلز</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>#1: سند صرف - مقاس A4 - أصل فقط - طباعة ديجيتال | Qty: 500 | Price: .75 | Total: 375 | VAT: 56.25</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>375</v>
+      </c>
+      <c r="F180" t="n">
+        <v>56.25</v>
+      </c>
+      <c r="G180" t="n">
+        <v>431.25</v>
+      </c>
+      <c r="I180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>أجاد</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>#1: استيكر العود الأزرق - شفاف - مقاس 3.5*4.5 سم | Qty: 240 | Price: 0.67 | Total: 160.8 | VAT: 0; #2: استيكر الشعار - شفاف - دائري - مقاس 6*6 سم | Qty: 240 | Price: .96 | Total: 230.39999999999998 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>391.2</v>
+      </c>
+      <c r="F181" t="n">
+        <v>0</v>
+      </c>
+      <c r="G181" t="n">
+        <v>391.2</v>
+      </c>
+      <c r="I181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>عبدالإله الكعكي</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>#1: ختم مؤسسة إبراهيم عبدالغني R538 | Qty: 1 | Price: 115 | Total: 115 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>115</v>
+      </c>
+      <c r="F182" t="n">
+        <v>0</v>
+      </c>
+      <c r="G182" t="n">
+        <v>115</v>
+      </c>
+      <c r="I182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>أبراج اللؤلؤة</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>#1: سند صرف لون واحد (أزرق بحري) - 1+2 - ترقيم 501 | Qty: 10 | Price: 20 | Total: 200 | VAT: 30</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>200</v>
+      </c>
+      <c r="F183" t="n">
+        <v>30</v>
+      </c>
+      <c r="G183" t="n">
+        <v>230</v>
+      </c>
+      <c r="I183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>مجموعة سدر</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>#1: لوحة أكريليك مقاس 37*27 سم - 6ملم مطبوع من الخلف | Qty: 1 | Price: 120 | Total: 120 | VAT: 18</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Invoice#375, QB#5147</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>120</v>
+      </c>
+      <c r="F184" t="n">
+        <v>18</v>
+      </c>
+      <c r="G184" t="n">
+        <v>138</v>
+      </c>
+      <c r="I184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>أم عبدالمحسن</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>#1: طباعة ديجيتال - جيب بطاقة لظرف القهوة - مقاس 13*12 سم مقفل - سماكة 150 جرام | Qty: 100 | Price: 2.5 | Total: 250 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>QB#5145</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>250</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0</v>
+      </c>
+      <c r="G185" t="n">
+        <v>250</v>
+      </c>
+      <c r="I185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>مؤسسة حرير البحر</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>#1: ختم مستطيل S827 | Qty: 1 | Price: 138 | Total: 138 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>QB#5149</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>138</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0</v>
+      </c>
+      <c r="G186" t="n">
+        <v>138</v>
+      </c>
+      <c r="I186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>مسجد محطة السليمانية</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>#1: لوحة أكريليك مفرغة مع بخاخ بوية لون أزرق | Qty: 1 | Price: 250 | Total: 250 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>250</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0</v>
+      </c>
+      <c r="G187" t="n">
+        <v>250</v>
+      </c>
+      <c r="I187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>مركز كنوز الطفولة</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>#1: بنر مقاس 150*100 سم | Qty: 3 | Price: 60 | Total: 180 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>QB#5148</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>180</v>
+      </c>
+      <c r="F188" t="n">
+        <v>0</v>
+      </c>
+      <c r="G188" t="n">
+        <v>180</v>
+      </c>
+      <c r="I188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>زكي نبيل</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>#1: فلين مقاس 45*65 سم | Qty: 1 | Price: 57.5 | Total: 57.5 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>QB#5146</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="F189" t="n">
+        <v>0</v>
+      </c>
+      <c r="G189" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="I189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>شركة المورد والإمداد</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>#1: استيكر بلاستيك - مقاس 30*20 سم | Qty: 500 | Price: 1.4 | Total: 700 | VAT: 105</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Invoice#377</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>700</v>
+      </c>
+      <c r="F190" t="n">
+        <v>105</v>
+      </c>
+      <c r="G190" t="n">
+        <v>805</v>
+      </c>
+      <c r="I190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>علي عمر دين</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>#1: استيكر الدليل التجاري - طباعة ديجيتال - مقاس 9.5*15.5 سم | Qty: 200 | Price: .5 | Total: 100 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>QB#5158</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>100</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0</v>
+      </c>
+      <c r="G191" t="n">
+        <v>100</v>
+      </c>
+      <c r="I191" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>مجمع قبل وبعد</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>#1: فلين 50*70 سم | Qty: 1 | Price: 40 | Total: 40 | VAT: 6</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>40</v>
+      </c>
+      <c r="F192" t="n">
+        <v>6</v>
+      </c>
+      <c r="G192" t="n">
+        <v>46</v>
+      </c>
+      <c r="I192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>رانيا بن محفوظ</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>#1: استيكر بلاستيك مقاس 70*100 سم - مركب على ورق مقوى | Qty: 1 | Price: 80 | Total: 80 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>80</v>
+      </c>
+      <c r="F193" t="n">
+        <v>0</v>
+      </c>
+      <c r="G193" t="n">
+        <v>80</v>
+      </c>
+      <c r="I193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>قرطاسية المودة</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>#1: رول اب مطبوع على بنر | Qty: 1 | Price: 150 | Total: 150 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>150</v>
+      </c>
+      <c r="F194" t="n">
+        <v>0</v>
+      </c>
+      <c r="G194" t="n">
+        <v>150</v>
+      </c>
+      <c r="I194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>ندى - كروت اليوم الوطني</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>#1: كروت ثيم اليوم الوطني مقاس 10*9 سم - نموذجين - ألف من كل نموذج | Qty: 2000 | Price: .20 | Total: 400 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>400</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0</v>
+      </c>
+      <c r="G195" t="n">
+        <v>400</v>
+      </c>
+      <c r="I195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>نادي الاتحاد</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>#1: لوحة فوركس مقاس A4 - مع قاعدة أكريليك مطبوعة يو في | Qty: 2 | Price: 100 | Total: 200 | VAT: 30; #2: لوحة فوركس مقاس A5 - مع قاعدة أكريليك مطبوعة يو في | Qty: 2 | Price: 70 | Total: 140 | VAT: 21</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>340</v>
+      </c>
+      <c r="F196" t="n">
+        <v>51</v>
+      </c>
+      <c r="G196" t="n">
+        <v>391</v>
+      </c>
+      <c r="I196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>فارس البلوشي</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>#1: درع كريستال | Qty: 1 | Price: 161 | Total: 161 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>161</v>
+      </c>
+      <c r="F197" t="n">
+        <v>0</v>
+      </c>
+      <c r="G197" t="n">
+        <v>161</v>
+      </c>
+      <c r="I197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>شاي فال</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>#1: استيكرات الأكواب | Qty: 10000 | Price: .25 | Total: 2500 | VAT: 375</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F198" t="n">
+        <v>375</v>
+      </c>
+      <c r="G198" t="n">
+        <v>2875</v>
+      </c>
+      <c r="I198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>عبدالله باقيس</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>#1: رول أب - طباعة على بنر | Qty: 1 | Price: 230 | Total: 230 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>230</v>
+      </c>
+      <c r="F199" t="n">
+        <v>0</v>
+      </c>
+      <c r="G199" t="n">
+        <v>230</v>
+      </c>
+      <c r="I199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>دكتور فهد باحارثة</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>#1: كوبونات كالعادة | Qty: 1000 | Price: .41 | Total: 410 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>410</v>
+      </c>
+      <c r="F200" t="n">
+        <v>0</v>
+      </c>
+      <c r="G200" t="n">
+        <v>410</v>
+      </c>
+      <c r="I200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>دكتورة براء</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>#1: استيكر مقاس 15*10 سم - طباعة ديجيتال | Qty: 100 | Price: 1.04 | Total: 104 | VAT: 0; #2: استيكر مقاس 18*4 سم - طباعة ديجيتال | Qty: 100 | Price: .92 | Total: 92 | VAT: 0; #3: استيكر مقاس 13*7 سم - طباعة ديجيتال | Qty: 100 | Price: .92 | Total: 92 | VAT: 0; #4: استيكر مقاس 9*4 سم - طباعة ديجيتال | Qty: 100 | Price: .92 | Total: 92 | VAT: 0; #5: استيكر بلاستيك مقاس 5*5 سم | Qty: 100 | Price: .92 | Total: 92 | VAT: 0; #6: طباعة كرت مقاس 15*10 سم | Qty: 100 | Price: 1.15 | Total: 114.99999999999999 | VAT: 0</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>587</v>
+      </c>
+      <c r="F201" t="n">
+        <v>0</v>
+      </c>
+      <c r="G201" t="n">
+        <v>587</v>
+      </c>
+      <c r="I201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>شركة متحدة الأعمال</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>#1: ختم S827 | Qty: 1 | Price: 100 | Total: 100 | VAT: 15</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>100</v>
+      </c>
+      <c r="F202" t="n">
+        <v>15</v>
+      </c>
+      <c r="G202" t="n">
+        <v>115</v>
+      </c>
+      <c r="I202" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5470,7 +6813,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5824,7 +7167,6 @@
           <t>bank</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
       <c r="G14" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Show discount in expanded sales transaction row. Discount now visible in UI for each transaction. Minor UI improvement.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I202"/>
+  <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
       <selection activeCell="A177" sqref="A177:XFD178"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>#1: استيكر مقاس 5.5*13.5 سم - طباعة ديجيتال | Qty: 100 | Price: 1.03 | Total: 103 | VAT: 0; #2: سليف علبة - طباعة ورق 150 جرام - مقاس 21*6.5 سم | Qty: 100 | Price: 2.07 | Total: 207 | VAT: 0; #3: تسوية الضريبة | Qty: 1 | Price: 0.5 | Total: 0.5 | VAT: 0</t>
+          <t>#1: استيكر مقاس 5.5*13.5 سم - طباعة ديجيتال | Qty: 100 | Price: 1.03 | Total: 103 | VAT: 0; #2: سليف علبة - طباعة ورق 150 جرام - مقاس 21*6.5 سم | Qty: 100 | Price: 2.07 | Total: 207 | VAT: 0; #3: تسوية الضريبة | Qty: 1 | Price: 0.5 | Total: 0.5 | VAT: 0; Discount: 0</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -5157,7 +5157,7 @@
         <v>310.5</v>
       </c>
       <c r="I150" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>#1: توريد وطباعة أكياس ورقية - مقاس A5 | Qty: 100 | Price: 3.45 | Total: 345 | VAT: 0; #2: استيكر مقاس 5*5 سم - دائري | Qty: 100 | Price: .69 | Total: 69 | VAT: 0</t>
+          <t>#1: توريد وطباعة أكياس ورقية - مقاس A5 | Qty: 100 | Price: 3.45 | Total: 345 | VAT: 0; #2: استيكر مقاس 5*5 سم - دائري | Qty: 100 | Price: .69 | Total: 69 | VAT: 0; Discount: 0</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -5190,8 +5190,9 @@
       <c r="G151" t="n">
         <v>414</v>
       </c>
+      <c r="H151" t="inlineStr"/>
       <c r="I151" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -5304,12 +5305,16 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>#1: استيكر الأدهم - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.745 | Total: 74.5 | VAT: 0; #2: استيكر الكميت - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.745 | Total: 74.5 | VAT: 0; #3: استيكر مقاس 5.5*5.5 سم - دائري | Qty: 200 | Price: 0.805 | Total: 161 | VAT: 0; #4: كرت طريقة الاستخدام - كوشيه مسلفن مطفي - مقاس A6 - طباعة وجهين | Qty: 500 | Price: 0.506 | Total: 253 | VAT: 0</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr"/>
+          <t>#1: استيكر الأدهم - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.747 | Total: 74.7 | VAT: 0; #2: استيكر الكميت - شفاف - مقاس 3*2 سم | Qty: 100 | Price: 0.748 | Total: 74.8 | VAT: 0; #3: استيكر مقاس 5.5*5.5 سم - دائري | Qty: 200 | Price: 0.805 | Total: 161 | VAT: 0; #4: كرت طريقة الاستخدام - كوشيه مسلفن مطفي - مقاس A6 - طباعة وجهين | Qty: 500 | Price: 0.506 | Total: 253 | VAT: 0; Discount: 13.5</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>QB#5168</t>
+        </is>
+      </c>
       <c r="E155" t="n">
-        <v>563</v>
+        <v>563.5</v>
       </c>
       <c r="F155" t="n">
         <v>0</v>
@@ -5317,7 +5322,6 @@
       <c r="G155" t="n">
         <v>550</v>
       </c>
-      <c r="H155" t="inlineStr"/>
       <c r="I155" t="b">
         <v>0</v>
       </c>
@@ -5335,20 +5339,25 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>#1: ختم دائري مقاس R538 | Qty: 1 | Price: 115 | Total: 115 | VAT: 0</t>
+          <t>#1: ختم دائري مقاس R538 | Qty: 1 | Price: 100 | Total: 100 | VAT: 15; Discount: 0</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Invoice#365, QB#5169</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F156" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G156" t="n">
         <v>115</v>
       </c>
       <c r="I156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -5733,7 +5742,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>#1: استيكر مقاس 60*12 سم | Qty: 2 | Price: 20 | Total: 40 | VAT: 0; #2: استيكر مقاس 44*7 سم | Qty: 1 | Price: 10 | Total: 10 | VAT: 0</t>
+          <t>#1: استيكر مقاس 60*12 سم | Qty: 2 | Price: 30 | Total: 60 | VAT: 0; #2: استيكر مقاس 44*7 سم | Qty: 1 | Price: 20 | Total: 20 | VAT: 0; Discount: 0</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5742,16 +5751,16 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F168" t="n">
         <v>0</v>
       </c>
       <c r="G168" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -6797,6 +6806,122 @@
         <v>115</v>
       </c>
       <c r="I202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>دوت وان كافيه</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>#1: رول أب على خامة بنر مقاس 85*200 سم | Qty: 3 | Price: 200 | Total: 600 | VAT: 90; Discount: 0</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>600</v>
+      </c>
+      <c r="F203" t="n">
+        <v>90</v>
+      </c>
+      <c r="G203" t="n">
+        <v>690</v>
+      </c>
+      <c r="I203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>أبراج اللؤلؤة</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>2025-08-23</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>#1: ختم دائري R538 | Qty: 1 | Price: 120 | Total: 120 | VAT: 18; Discount: 0</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>120</v>
+      </c>
+      <c r="F204" t="n">
+        <v>18</v>
+      </c>
+      <c r="G204" t="n">
+        <v>138</v>
+      </c>
+      <c r="I204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>خالد أبو سعيد</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>2025-08-23</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>#1: استيكرات المنتجات | Qty: 1 | Price:  | Total: 0 | VAT: 0; Discount: 0</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>0</v>
+      </c>
+      <c r="F205" t="n">
+        <v>0</v>
+      </c>
+      <c r="G205" t="n">
+        <v>0</v>
+      </c>
+      <c r="I205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>أسامة الأحمدي</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>2025-08-23</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>#1: رول أب مع مكينة - طباعة بنر - مقاس 85*200 سم | Qty: 1 | Price: 170 | Total: 170 | VAT: 0; #2: بنر مقاس 80*140 سم | Qty: 1 | Price: 50 | Total: 50 | VAT: 0; #3: بنر مقاس 120*160 سم | Qty: 1 | Price: 70 | Total: 70 | VAT: 0; Discount: 0</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>290</v>
+      </c>
+      <c r="F206" t="n">
+        <v>0</v>
+      </c>
+      <c r="G206" t="n">
+        <v>290</v>
+      </c>
+      <c r="I206" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>